<commit_message>
CSS3 - Transform / video 11
</commit_message>
<xml_diff>
--- a/CSS3.xlsx
+++ b/CSS3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D092C004-7DF6-44F6-89CF-74591549CB69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82855E0D-81AE-4CE5-BDC6-7C549913C2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>هاي معناته من كل الجهات عشره بكسل تدوير للحواف</t>
   </si>
@@ -403,6 +403,76 @@
   </si>
   <si>
     <t>هذا يفر العنصر حسب الدرجه المراده</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>transform: scale(2,2)</t>
+  </si>
+  <si>
+    <t>transform: scale(2)</t>
+  </si>
+  <si>
+    <t>transform: scaleX(2)</t>
+  </si>
+  <si>
+    <t>transform: scaleY(2)</t>
+  </si>
+  <si>
+    <t>transform: none</t>
+  </si>
+  <si>
+    <t>هذا الامر حته تغير بحجم عنصر معين جان عنده ابعاد اصلا
+الرقم الاول الطول والثاني يمثل العرض</t>
+  </si>
+  <si>
+    <t>اذا تكتب بين القوسين رقم واحد ,, فهذا يعني انو التغير يصير بنفس القيمه
+عالطول والعرض</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الاكس تعني العرض </t>
+  </si>
+  <si>
+    <t>الواي تعني الطول</t>
+  </si>
+  <si>
+    <t>تلغي الخاصيه</t>
+  </si>
+  <si>
+    <t>Translate</t>
+  </si>
+  <si>
+    <t>transform: translate(10px, 20px)</t>
+  </si>
+  <si>
+    <t>transform: translate(10px, 0px)</t>
+  </si>
+  <si>
+    <t>transform: translate(10px)</t>
+  </si>
+  <si>
+    <t>transform: translateX(10px)</t>
+  </si>
+  <si>
+    <t>transform: translateY(10px)</t>
+  </si>
+  <si>
+    <t>هذا الامر حته تحرك العناصر بنسب معينه,, الرقم الاول يحرك عرضيا
+والثاني يحرك طوليا</t>
+  </si>
+  <si>
+    <t>اذا تريد تحرك من جهه وحده هيج تسوي</t>
+  </si>
+  <si>
+    <t>اذا تكتب قيمه وحده يعتربها عرضيا مو مثل السكيل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هاي علمود تحرك بس عرضيا </t>
+  </si>
+  <si>
+    <t>وهاي حته تحرك بس طوليا
+هاي الخواص تقبل قيم سالبه</t>
   </si>
 </sst>
 </file>
@@ -535,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -570,6 +640,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -1080,7 +1165,7 @@
       </c>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="16" t="s">
         <v>46</v>
       </c>
@@ -1088,7 +1173,98 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="25.8" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="1:2" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
+      <c r="A32" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="46.2" x14ac:dyDescent="0.45">
+      <c r="A33" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
+      <c r="A38" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="93.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CSS3 - Transform /3D
</commit_message>
<xml_diff>
--- a/CSS3.xlsx
+++ b/CSS3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82855E0D-81AE-4CE5-BDC6-7C549913C2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0171239-782E-4619-BCAF-7074A99B0134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>هاي معناته من كل الجهات عشره بكسل تدوير للحواف</t>
   </si>
@@ -402,9 +402,6 @@
     </r>
   </si>
   <si>
-    <t>هذا يفر العنصر حسب الدرجه المراده</t>
-  </si>
-  <si>
     <t>Scale</t>
   </si>
   <si>
@@ -437,9 +434,6 @@
     <t>الواي تعني الطول</t>
   </si>
   <si>
-    <t>تلغي الخاصيه</t>
-  </si>
-  <si>
     <t>Translate</t>
   </si>
   <si>
@@ -473,13 +467,67 @@
   <si>
     <t>وهاي حته تحرك بس طوليا
 هاي الخواص تقبل قيم سالبه</t>
+  </si>
+  <si>
+    <t>Skew</t>
+  </si>
+  <si>
+    <t>transform: skew(10deg, 20deg)</t>
+  </si>
+  <si>
+    <t>transform: skew(10px, 0px)</t>
+  </si>
+  <si>
+    <t>transform: skew(10px)</t>
+  </si>
+  <si>
+    <t>transform: skewX(10px)</t>
+  </si>
+  <si>
+    <t>transform: skewY(10px)</t>
+  </si>
+  <si>
+    <t>هذا الامر حته  تحرف العناصر بنسب معينه,, الرقم الاول يحرف عرضيا
+والثاني يحرف طوليا</t>
+  </si>
+  <si>
+    <t>هاي اذا تريد تحرف من جهه وحده</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هاي علمود تحرف بس عرضيا </t>
+  </si>
+  <si>
+    <t>وهاي حته تحرف بس طوليا
+هاي الخواص تقبل قيم سالبه</t>
+  </si>
+  <si>
+    <t>تلغي الخاصيه
+ملاحظه  ,, ممكن تسوي flip للعنصر سواء عمودي او افقي عن طريق
+تخلي القيمتين متعاكسات بالاشاره</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">هذا يفر العنصر حسب الدرجه المراده
+ملاحظه ,, ممكن يقبل قيم سالبه ,, وممكن نخلي </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>rotateX or Y or Z</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +593,14 @@
       <color rgb="FF00B050"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -941,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -1165,104 +1221,150 @@
       </c>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:2" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>47</v>
+      <c r="B30" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="7"/>
     </row>
     <row r="32" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
       <c r="A32" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="46.2" x14ac:dyDescent="0.45">
       <c r="A33" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
       <c r="A38" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="93.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="12" t="s">
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
+      <c r="A44" s="17" t="s">
         <v>69</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CSS3 - Video /18
</commit_message>
<xml_diff>
--- a/CSS3.xlsx
+++ b/CSS3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0171239-782E-4619-BCAF-7074A99B0134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BDFB4C-1247-4F2E-A06B-CE666FBF5392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>هاي معناته من كل الجهات عشره بكسل تدوير للحواف</t>
   </si>
@@ -521,6 +521,19 @@
       </rPr>
       <t>rotateX or Y or Z</t>
     </r>
+  </si>
+  <si>
+    <t>transform: scale3D(1.2, 1.5, 2)</t>
+  </si>
+  <si>
+    <t>transform: scaleZ(2)</t>
+  </si>
+  <si>
+    <t>هاي نفس الفوكاها بس نختصر نكتب بس زي معناته البعد الثالث</t>
+  </si>
+  <si>
+    <t>هيج نسوي سكيل بالبعد الثالث بس البعد الثالث ميبين الا اكو وياه  فد نوع 
+ترانسفورم ثاني مثل روتيت او ترانسلايت</t>
   </si>
 </sst>
 </file>
@@ -603,7 +616,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,8 +635,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -657,11 +676,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -711,6 +739,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -1267,103 +1301,119 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B38" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="6" t="s">
+    <row r="39" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="7"/>
-    </row>
-    <row r="38" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
-      <c r="A38" s="17" t="s">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
+      <c r="A40" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B40" s="18" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B43" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="4" t="s">
+    <row r="44" spans="1:2" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="6" t="s">
+    <row r="45" spans="1:2" ht="25.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="7"/>
-    </row>
-    <row r="44" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
-      <c r="A44" s="17" t="s">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:2" ht="45.6" x14ac:dyDescent="0.45">
+      <c r="A46" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B49" s="21" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="4" t="s">
+    <row r="50" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
will move to acer pc
</commit_message>
<xml_diff>
--- a/CSS3.xlsx
+++ b/CSS3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF9AEDF-CA7D-447F-ACAF-3F2C8CAC965C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93B815B-DD15-42FA-95E0-CDF2F0F1C1F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Flex" sheetId="2" r:id="rId2"/>
     <sheet name="Grid" sheetId="3" r:id="rId3"/>
+    <sheet name="Transition" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="179">
   <si>
     <t>هاي معناته من كل الجهات عشره بكسل تدوير للحواف</t>
   </si>
@@ -1010,12 +1011,72 @@
       <t>y</t>
     </r>
   </si>
+  <si>
+    <t>transition-duration</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>1000ms</t>
+  </si>
+  <si>
+    <t>transition-delay</t>
+  </si>
+  <si>
+    <t>transition-property</t>
+  </si>
+  <si>
+    <t>width;</t>
+  </si>
+  <si>
+    <t>width, height</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>transition-timing-function</t>
+  </si>
+  <si>
+    <t>ease</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>ease-in</t>
+  </si>
+  <si>
+    <t>ease-out</t>
+  </si>
+  <si>
+    <t>ease-in-out</t>
+  </si>
+  <si>
+    <t>transition:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All 2s 1s linear  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>shorthand</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1179,8 +1240,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1220,6 +1309,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1406,6 +1501,21 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2308,7 +2418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EF259E-1D95-436F-9324-5FC6AACCD2DF}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2500,4 +2610,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046C8E51-F823-45C4-8863-F9A133840042}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="37.1796875" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.36328125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="25.08984375" style="48" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="50" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="37.1796875" style="48"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>